<commit_message>
add router and link for header
</commit_message>
<xml_diff>
--- a/material/assignment.xlsx
+++ b/material/assignment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\leminhshop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\leminhshop\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F355C1-7DB2-42C8-971D-43E78AB431CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA28086E-5AF7-4EF3-B82D-4E682E093C76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>leminhshop Project (HCI relearn course)</t>
   </si>
@@ -45,9 +45,6 @@
     <t>https://github.com/tieuminhminh/leminhshop.git</t>
   </si>
   <si>
-    <t>backend,logic</t>
-  </si>
-  <si>
     <t>Minh</t>
   </si>
   <si>
@@ -63,21 +60,12 @@
     <t>manage category</t>
   </si>
   <si>
-    <t>manage user</t>
-  </si>
-  <si>
     <t>manage file</t>
   </si>
   <si>
     <t>manage order</t>
   </si>
   <si>
-    <t>manage cart</t>
-  </si>
-  <si>
-    <t>payment</t>
-  </si>
-  <si>
     <t>user sites</t>
   </si>
   <si>
@@ -87,19 +75,61 @@
     <t>register</t>
   </si>
   <si>
-    <t>all html page in bstore</t>
-  </si>
-  <si>
-    <t>delete unnecessary element</t>
-  </si>
-  <si>
     <t>admin sites</t>
   </si>
   <si>
     <t>Hằng</t>
   </si>
   <si>
-    <t>8/4/2020</t>
+    <t>show product</t>
+  </si>
+  <si>
+    <t>view cart</t>
+  </si>
+  <si>
+    <t>payment method</t>
+  </si>
+  <si>
+    <t>shipping</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>contact us</t>
+  </si>
+  <si>
+    <t>about us</t>
+  </si>
+  <si>
+    <t>manage post</t>
+  </si>
+  <si>
+    <t>manage account</t>
+  </si>
+  <si>
+    <t>manage role</t>
+  </si>
+  <si>
+    <t>manage order process</t>
+  </si>
+  <si>
+    <t>manage check out</t>
+  </si>
+  <si>
+    <t>manage shipping</t>
+  </si>
+  <si>
+    <t>manage coupon</t>
+  </si>
+  <si>
+    <t>manage profile</t>
+  </si>
+  <si>
+    <t>manage promotion</t>
+  </si>
+  <si>
+    <t>manage tax</t>
   </si>
 </sst>
 </file>
@@ -285,65 +315,65 @@
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -626,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -642,211 +672,245 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="10"/>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+      <c r="B5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="10"/>
+      <c r="B6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="21"/>
+      <c r="B9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="17"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
+      <c r="B12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
+      <c r="B13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
+      <c r="B15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+      <c r="B16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="13"/>
+      <c r="B17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="14"/>
+      <c r="B18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="18"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="13"/>
+      <c r="B20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="13"/>
+      <c r="B21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="13"/>
+      <c r="B22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="13"/>
+      <c r="B23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="13"/>
+      <c r="B24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="18">
-        <v>44047</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
-      <c r="B9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="17"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="20"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="20"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="21"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="18">
-        <v>44047</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
-      <c r="B17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
-      <c r="B18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="16"/>
-      <c r="B20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="14"/>
+      <c r="B25" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="A14:A20"/>
-    <mergeCell ref="D3:D9"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="D14:D20"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C3:C9"/>
     <mergeCell ref="A3:A9"/>
+    <mergeCell ref="C10:C18"/>
+    <mergeCell ref="A10:A18"/>
+    <mergeCell ref="C19:C25"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="D3:D9"/>
+    <mergeCell ref="D10:D18"/>
+    <mergeCell ref="D19:D25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>